<commit_message>
Added comments and replaced SimpleXSLX with phpspreadsheet
</commit_message>
<xml_diff>
--- a/assets/spreadsheets/template/TIME_SHEET_SUMMARY.xlsx
+++ b/assets/spreadsheets/template/TIME_SHEET_SUMMARY.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\PhpTrial\assets\spreadsheets\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B19B09A-EFB0-4B43-A113-2A81A264B8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EBCE3B-BB87-4D93-8B1F-C237FBB55920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{7A662600-E61D-454A-A014-CFB3ABF949DC}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{7A662600-E61D-454A-A014-CFB3ABF949DC}"/>
   </bookViews>
   <sheets>
     <sheet name="INTERN_ID" sheetId="1" r:id="rId1"/>
@@ -191,7 +191,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -212,6 +211,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -532,7 +534,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,128 +546,128 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="A16" s="9"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="9"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>